<commit_message>
Added several images. Modified themes. Implemented three new themes : Dark, Normal, Mild
</commit_message>
<xml_diff>
--- a/__RESOURCES/HaleyIcons_Set02/resourcegenerator.xlsx
+++ b/__RESOURCES/HaleyIcons_Set02/resourcegenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886933D6-FBD5-4D26-A13E-E5A8F6FF9C91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FE8A7A-1E05-47B9-B074-3AE304CA014C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="-96" windowWidth="22206" windowHeight="13152" xr2:uid="{860B0934-854C-4523-ACE3-F6AFFDA77800}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -130,6 +130,249 @@
   </si>
   <si>
     <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\tick_sharp_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender_clock.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender_clock_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender_clock_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\calender_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart_line.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart_line_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart_line_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\cart_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car_2.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car_2_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car_2_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\car_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\edit.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\edit_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\edit_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\firstaid.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\firstaid_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\firstaid_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag_triangle.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag_triangle_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\flag_triangle_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\gift.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\gift_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\gift_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_2.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_2_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_2_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_stand.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_stand_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\globe_stand_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home_2.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home_2_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home_2_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\home_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\medical.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\medical_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\medical_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\package.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\package_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\package_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\pen.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\pen_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\pen_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane_moving.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane_moving_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\plane_moving_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\suitcase.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\suitcase_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\suitcase_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\touch.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\touch_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\touch_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in_line.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in_line_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in_line_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_in_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out_line.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out_line_large.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out_line_medium.png</t>
+  </si>
+  <si>
+    <t>C:\Users\Lingam\source\repos\rmsmech\HaleyWPF\__RESOURCES\HaleyIcons_Set02\zoom_out_medium.png</t>
   </si>
 </sst>
 </file>
@@ -492,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434771DF-3FE8-45DE-8F64-EA44E95D1E20}">
   <dimension ref="A1:F194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="E114" sqref="E10:E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -860,1652 +1103,1895 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" ref="C25:C28" si="7" xml:space="preserve"> MID(A25,$B$6,(LEN(A25)-$B$10+1))</f>
-        <v>eye.png</v>
+        <v>calender.png</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" ref="D25:D28" si="8">LEFT(C25,LEN(C25)-4)</f>
-        <v>eye</v>
+        <v>calender</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" ref="E25:E28" si="9">D25&amp;","</f>
-        <v>eye,</v>
+        <v>calender,</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" ref="F25:F28" si="10">$A$1&amp;D25&amp;$A$2&amp;C25&amp;$A$3</f>
-        <v>&lt;ImageSource x:Key="eye"&gt;pack://application:,,,/Haley.WPF;component/Images/eye.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender"&gt;pack://application:,,,/Haley.WPF;component/Images/calender.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="7"/>
-        <v>eye_large.png</v>
+        <v>calender_clock.png</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="8"/>
-        <v>eye_large</v>
+        <v>calender_clock</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="9"/>
-        <v>eye_large,</v>
+        <v>calender_clock,</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;ImageSource x:Key="eye_large"&gt;pack://application:,,,/Haley.WPF;component/Images/eye_large.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender_clock"&gt;pack://application:,,,/Haley.WPF;component/Images/calender_clock.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="7"/>
-        <v>eye_medium.png</v>
+        <v>calender_clock_large.png</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="8"/>
-        <v>eye_medium</v>
+        <v>calender_clock_large</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="9"/>
-        <v>eye_medium,</v>
+        <v>calender_clock_large,</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;ImageSource x:Key="eye_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/eye_medium.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender_clock_large"&gt;pack://application:,,,/Haley.WPF;component/Images/calender_clock_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="7"/>
-        <v>tick.png</v>
+        <v>calender_clock_medium.png</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="8"/>
-        <v>tick</v>
+        <v>calender_clock_medium</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="9"/>
-        <v>tick,</v>
+        <v>calender_clock_medium,</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="10"/>
-        <v>&lt;ImageSource x:Key="tick"&gt;pack://application:,,,/Haley.WPF;component/Images/tick.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender_clock_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/calender_clock_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" ref="C29:C92" si="11" xml:space="preserve"> MID(A29,$B$6,(LEN(A29)-$B$10+1))</f>
-        <v>tick_large.png</v>
+        <v>calender_large.png</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" ref="D29:D92" si="12">LEFT(C29,LEN(C29)-4)</f>
-        <v>tick_large</v>
+        <v>calender_large</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" ref="E29:E92" si="13">D29&amp;","</f>
-        <v>tick_large,</v>
+        <v>calender_large,</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" ref="F29:F92" si="14">$A$1&amp;D29&amp;$A$2&amp;C29&amp;$A$3</f>
-        <v>&lt;ImageSource x:Key="tick_large"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_large.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender_large"&gt;pack://application:,,,/Haley.WPF;component/Images/calender_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="11"/>
-        <v>tick_medium.png</v>
+        <v>calender_medium.png</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="12"/>
-        <v>tick_medium</v>
+        <v>calender_medium</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="13"/>
-        <v>tick_medium,</v>
+        <v>calender_medium,</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;ImageSource x:Key="tick_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_medium.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="calender_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/calender_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="11"/>
-        <v>tick_sharp.png</v>
+        <v>car.png</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="12"/>
-        <v>tick_sharp</v>
+        <v>car</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="13"/>
-        <v>tick_sharp,</v>
+        <v>car,</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;ImageSource x:Key="tick_sharp"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="car"&gt;pack://application:,,,/Haley.WPF;component/Images/car.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="11"/>
-        <v>tick_sharp_large.png</v>
+        <v>cart.png</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="12"/>
-        <v>tick_sharp_large</v>
+        <v>cart</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="13"/>
-        <v>tick_sharp_large,</v>
+        <v>cart,</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;ImageSource x:Key="tick_sharp_large"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp_large.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="cart"&gt;pack://application:,,,/Haley.WPF;component/Images/cart.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="11"/>
-        <v>tick_sharp_medium.png</v>
+        <v>cart_large.png</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="12"/>
-        <v>tick_sharp_medium</v>
+        <v>cart_large</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="13"/>
-        <v>tick_sharp_medium,</v>
+        <v>cart_large,</v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="14"/>
-        <v>&lt;ImageSource x:Key="tick_sharp_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp_medium.png&lt;/ImageSource&gt;</v>
+        <v>&lt;ImageSource x:Key="cart_large"&gt;pack://application:,,,/Haley.WPF;component/Images/cart_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
       <c r="C34" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D34" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E34" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F34" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>cart_line.png</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="12"/>
+        <v>cart_line</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="13"/>
+        <v>cart_line,</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="cart_line"&gt;pack://application:,,,/Haley.WPF;component/Images/cart_line.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
       <c r="C35" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D35" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E35" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F35" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>cart_line_large.png</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="12"/>
+        <v>cart_line_large</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="13"/>
+        <v>cart_line_large,</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="cart_line_large"&gt;pack://application:,,,/Haley.WPF;component/Images/cart_line_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
       <c r="C36" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D36" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E36" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F36" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>cart_line_medium.png</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="12"/>
+        <v>cart_line_medium</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="13"/>
+        <v>cart_line_medium,</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="cart_line_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/cart_line_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
       <c r="C37" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D37" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E37" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F37" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>cart_medium.png</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="12"/>
+        <v>cart_medium</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="13"/>
+        <v>cart_medium,</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="cart_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/cart_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
       <c r="C38" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D38" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E38" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F38" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>car_2.png</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="12"/>
+        <v>car_2</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="13"/>
+        <v>car_2,</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="car_2"&gt;pack://application:,,,/Haley.WPF;component/Images/car_2.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
       <c r="C39" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D39" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E39" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F39" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>car_2_large.png</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="12"/>
+        <v>car_2_large</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="13"/>
+        <v>car_2_large,</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="car_2_large"&gt;pack://application:,,,/Haley.WPF;component/Images/car_2_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
       <c r="C40" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D40" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E40" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F40" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>car_2_medium.png</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="12"/>
+        <v>car_2_medium</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="13"/>
+        <v>car_2_medium,</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="car_2_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/car_2_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
       <c r="C41" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D41" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E41" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F41" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>car_large.png</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="12"/>
+        <v>car_large</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="13"/>
+        <v>car_large,</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="car_large"&gt;pack://application:,,,/Haley.WPF;component/Images/car_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
       <c r="C42" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D42" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E42" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F42" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>car_medium.png</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="12"/>
+        <v>car_medium</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="13"/>
+        <v>car_medium,</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="car_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/car_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
       <c r="C43" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D43" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E43" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F43" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>edit.png</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="12"/>
+        <v>edit</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="13"/>
+        <v>edit,</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="edit"&gt;pack://application:,,,/Haley.WPF;component/Images/edit.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
       <c r="C44" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D44" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E44" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F44" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>edit_large.png</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="12"/>
+        <v>edit_large</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="13"/>
+        <v>edit_large,</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="edit_large"&gt;pack://application:,,,/Haley.WPF;component/Images/edit_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
       <c r="C45" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D45" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E45" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F45" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>edit_medium.png</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="12"/>
+        <v>edit_medium</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="13"/>
+        <v>edit_medium,</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="edit_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/edit_medium.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>23</v>
+      </c>
       <c r="C46" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D46" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E46" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F46" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>eye.png</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="12"/>
+        <v>eye</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="13"/>
+        <v>eye,</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="eye"&gt;pack://application:,,,/Haley.WPF;component/Images/eye.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
       <c r="C47" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D47" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E47" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F47" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
+        <v>eye_large.png</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="12"/>
+        <v>eye_large</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="13"/>
+        <v>eye_large,</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="eye_large"&gt;pack://application:,,,/Haley.WPF;component/Images/eye_large.png&lt;/ImageSource&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
       <c r="C48" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D48" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E48" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F48" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>eye_medium.png</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="12"/>
+        <v>eye_medium</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="13"/>
+        <v>eye_medium,</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="eye_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/eye_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
       <c r="C49" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D49" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E49" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F49" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>firstaid.png</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="12"/>
+        <v>firstaid</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="13"/>
+        <v>firstaid,</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="firstaid"&gt;pack://application:,,,/Haley.WPF;component/Images/firstaid.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
       <c r="C50" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D50" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E50" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F50" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>firstaid_large.png</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="12"/>
+        <v>firstaid_large</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="13"/>
+        <v>firstaid_large,</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="firstaid_large"&gt;pack://application:,,,/Haley.WPF;component/Images/firstaid_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
       <c r="C51" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D51" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E51" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F51" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>firstaid_medium.png</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="12"/>
+        <v>firstaid_medium</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="13"/>
+        <v>firstaid_medium,</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="firstaid_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/firstaid_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
       <c r="C52" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D52" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E52" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F52" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag.png</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="12"/>
+        <v>flag</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="13"/>
+        <v>flag,</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag"&gt;pack://application:,,,/Haley.WPF;component/Images/flag.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
       <c r="C53" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D53" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E53" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F53" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag_large.png</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="12"/>
+        <v>flag_large</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="13"/>
+        <v>flag_large,</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag_large"&gt;pack://application:,,,/Haley.WPF;component/Images/flag_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
       <c r="C54" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D54" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E54" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F54" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag_medium.png</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="12"/>
+        <v>flag_medium</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="13"/>
+        <v>flag_medium,</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/flag_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
       <c r="C55" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D55" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E55" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F55" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag_triangle.png</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="12"/>
+        <v>flag_triangle</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="13"/>
+        <v>flag_triangle,</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag_triangle"&gt;pack://application:,,,/Haley.WPF;component/Images/flag_triangle.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
       <c r="C56" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D56" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E56" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F56" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag_triangle_large.png</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="12"/>
+        <v>flag_triangle_large</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="13"/>
+        <v>flag_triangle_large,</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag_triangle_large"&gt;pack://application:,,,/Haley.WPF;component/Images/flag_triangle_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
       <c r="C57" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D57" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E57" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F57" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>flag_triangle_medium.png</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="12"/>
+        <v>flag_triangle_medium</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="13"/>
+        <v>flag_triangle_medium,</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="flag_triangle_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/flag_triangle_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
       <c r="C58" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D58" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E58" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F58" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>gift.png</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="12"/>
+        <v>gift</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="13"/>
+        <v>gift,</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="gift"&gt;pack://application:,,,/Haley.WPF;component/Images/gift.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
       <c r="C59" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D59" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E59" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F59" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>gift_large.png</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="12"/>
+        <v>gift_large</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="13"/>
+        <v>gift_large,</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="gift_large"&gt;pack://application:,,,/Haley.WPF;component/Images/gift_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
       <c r="C60" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D60" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E60" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F60" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>gift_medium.png</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="12"/>
+        <v>gift_medium</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="13"/>
+        <v>gift_medium,</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="gift_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/gift_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
       <c r="C61" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D61" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E61" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F61" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe.png</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="12"/>
+        <v>globe</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="13"/>
+        <v>globe,</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe"&gt;pack://application:,,,/Haley.WPF;component/Images/globe.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
       <c r="C62" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D62" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E62" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F62" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_2.png</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_2</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_2,</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_2"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_2.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
       <c r="C63" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D63" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E63" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F63" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_2_large.png</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_2_large</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_2_large,</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_2_large"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_2_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
       <c r="C64" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D64" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E64" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F64" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_2_medium.png</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_2_medium</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_2_medium,</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_2_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_2_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
       <c r="C65" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D65" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E65" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F65" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_large.png</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_large</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_large,</v>
+      </c>
+      <c r="F65" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_large"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
       <c r="C66" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D66" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E66" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F66" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_medium.png</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_medium</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_medium,</v>
+      </c>
+      <c r="F66" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
       <c r="C67" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D67" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E67" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F67" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_stand.png</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_stand</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_stand,</v>
+      </c>
+      <c r="F67" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_stand"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_stand.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
       <c r="C68" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D68" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E68" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F68" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_stand_large.png</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_stand_large</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_stand_large,</v>
+      </c>
+      <c r="F68" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_stand_large"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_stand_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
       <c r="C69" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D69" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E69" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F69" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>globe_stand_medium.png</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="12"/>
+        <v>globe_stand_medium</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="13"/>
+        <v>globe_stand_medium,</v>
+      </c>
+      <c r="F69" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="globe_stand_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/globe_stand_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
       <c r="C70" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D70" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E70" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F70" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home.png</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="12"/>
+        <v>home</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="13"/>
+        <v>home,</v>
+      </c>
+      <c r="F70" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home"&gt;pack://application:,,,/Haley.WPF;component/Images/home.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
       <c r="C71" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D71" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E71" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F71" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home_2.png</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="12"/>
+        <v>home_2</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="13"/>
+        <v>home_2,</v>
+      </c>
+      <c r="F71" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home_2"&gt;pack://application:,,,/Haley.WPF;component/Images/home_2.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
       <c r="C72" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D72" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E72" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F72" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home_2_large.png</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="12"/>
+        <v>home_2_large</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="13"/>
+        <v>home_2_large,</v>
+      </c>
+      <c r="F72" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home_2_large"&gt;pack://application:,,,/Haley.WPF;component/Images/home_2_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
       <c r="C73" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D73" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E73" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F73" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home_2_medium.png</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="12"/>
+        <v>home_2_medium</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="13"/>
+        <v>home_2_medium,</v>
+      </c>
+      <c r="F73" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home_2_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/home_2_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
       <c r="C74" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D74" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E74" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F74" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home_large.png</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="12"/>
+        <v>home_large</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="13"/>
+        <v>home_large,</v>
+      </c>
+      <c r="F74" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home_large"&gt;pack://application:,,,/Haley.WPF;component/Images/home_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
       <c r="C75" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D75" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E75" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F75" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>home_medium.png</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="12"/>
+        <v>home_medium</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="13"/>
+        <v>home_medium,</v>
+      </c>
+      <c r="F75" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="home_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/home_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
       <c r="C76" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D76" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E76" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F76" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>medical.png</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="12"/>
+        <v>medical</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="13"/>
+        <v>medical,</v>
+      </c>
+      <c r="F76" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="medical"&gt;pack://application:,,,/Haley.WPF;component/Images/medical.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
       <c r="C77" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D77" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E77" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F77" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>medical_large.png</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="12"/>
+        <v>medical_large</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="13"/>
+        <v>medical_large,</v>
+      </c>
+      <c r="F77" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="medical_large"&gt;pack://application:,,,/Haley.WPF;component/Images/medical_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
       <c r="C78" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D78" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E78" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F78" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>medical_medium.png</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="12"/>
+        <v>medical_medium</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="13"/>
+        <v>medical_medium,</v>
+      </c>
+      <c r="F78" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="medical_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/medical_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
       <c r="C79" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D79" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E79" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F79" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>package.png</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="12"/>
+        <v>package</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="13"/>
+        <v>package,</v>
+      </c>
+      <c r="F79" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="package"&gt;pack://application:,,,/Haley.WPF;component/Images/package.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
       <c r="C80" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D80" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E80" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F80" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>package_large.png</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="12"/>
+        <v>package_large</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="13"/>
+        <v>package_large,</v>
+      </c>
+      <c r="F80" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="package_large"&gt;pack://application:,,,/Haley.WPF;component/Images/package_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
       <c r="C81" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D81" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E81" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F81" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>package_medium.png</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="12"/>
+        <v>package_medium</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="13"/>
+        <v>package_medium,</v>
+      </c>
+      <c r="F81" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="package_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/package_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
       <c r="C82" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D82" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E82" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F82" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>pen.png</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="12"/>
+        <v>pen</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="13"/>
+        <v>pen,</v>
+      </c>
+      <c r="F82" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="pen"&gt;pack://application:,,,/Haley.WPF;component/Images/pen.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
       <c r="C83" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D83" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E83" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F83" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>pen_large.png</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="12"/>
+        <v>pen_large</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="13"/>
+        <v>pen_large,</v>
+      </c>
+      <c r="F83" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="pen_large"&gt;pack://application:,,,/Haley.WPF;component/Images/pen_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
       <c r="C84" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D84" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E84" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F84" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>pen_medium.png</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="12"/>
+        <v>pen_medium</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="13"/>
+        <v>pen_medium,</v>
+      </c>
+      <c r="F84" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="pen_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/pen_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
       <c r="C85" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D85" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E85" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F85" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane.png</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="12"/>
+        <v>plane</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="13"/>
+        <v>plane,</v>
+      </c>
+      <c r="F85" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane"&gt;pack://application:,,,/Haley.WPF;component/Images/plane.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
       <c r="C86" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D86" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E86" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F86" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane_large.png</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="12"/>
+        <v>plane_large</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="13"/>
+        <v>plane_large,</v>
+      </c>
+      <c r="F86" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane_large"&gt;pack://application:,,,/Haley.WPF;component/Images/plane_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
       <c r="C87" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D87" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E87" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F87" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane_medium.png</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="12"/>
+        <v>plane_medium</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="13"/>
+        <v>plane_medium,</v>
+      </c>
+      <c r="F87" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/plane_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
       <c r="C88" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D88" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E88" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F88" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane_moving.png</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="12"/>
+        <v>plane_moving</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="13"/>
+        <v>plane_moving,</v>
+      </c>
+      <c r="F88" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane_moving"&gt;pack://application:,,,/Haley.WPF;component/Images/plane_moving.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
       <c r="C89" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D89" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E89" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F89" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane_moving_large.png</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="12"/>
+        <v>plane_moving_large</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="13"/>
+        <v>plane_moving_large,</v>
+      </c>
+      <c r="F89" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane_moving_large"&gt;pack://application:,,,/Haley.WPF;component/Images/plane_moving_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
       <c r="C90" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D90" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E90" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F90" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>plane_moving_medium.png</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="12"/>
+        <v>plane_moving_medium</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="13"/>
+        <v>plane_moving_medium,</v>
+      </c>
+      <c r="F90" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="plane_moving_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/plane_moving_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>95</v>
+      </c>
       <c r="C91" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D91" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E91" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F91" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>suitcase.png</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="12"/>
+        <v>suitcase</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="13"/>
+        <v>suitcase,</v>
+      </c>
+      <c r="F91" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="suitcase"&gt;pack://application:,,,/Haley.WPF;component/Images/suitcase.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
       <c r="C92" t="str">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="D92" t="e">
-        <f t="shared" si="12"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E92" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F92" t="e">
-        <f t="shared" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>suitcase_large.png</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="12"/>
+        <v>suitcase_large</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="13"/>
+        <v>suitcase_large,</v>
+      </c>
+      <c r="F92" t="str">
+        <f t="shared" si="14"/>
+        <v>&lt;ImageSource x:Key="suitcase_large"&gt;pack://application:,,,/Haley.WPF;component/Images/suitcase_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>97</v>
+      </c>
       <c r="C93" t="str">
         <f t="shared" ref="C93:C156" si="15" xml:space="preserve"> MID(A93,$B$6,(LEN(A93)-$B$10+1))</f>
-        <v/>
-      </c>
-      <c r="D93" t="e">
+        <v>suitcase_medium.png</v>
+      </c>
+      <c r="D93" t="str">
         <f t="shared" ref="D93:D156" si="16">LEFT(C93,LEN(C93)-4)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E93" t="e">
+        <v>suitcase_medium</v>
+      </c>
+      <c r="E93" t="str">
         <f t="shared" ref="E93:E156" si="17">D93&amp;","</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F93" t="e">
+        <v>suitcase_medium,</v>
+      </c>
+      <c r="F93" t="str">
         <f t="shared" ref="F93:F156" si="18">$A$1&amp;D93&amp;$A$2&amp;C93&amp;$A$3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>&lt;ImageSource x:Key="suitcase_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/suitcase_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>26</v>
+      </c>
       <c r="C94" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D94" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E94" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F94" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick.png</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="16"/>
+        <v>tick</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="17"/>
+        <v>tick,</v>
+      </c>
+      <c r="F94" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick"&gt;pack://application:,,,/Haley.WPF;component/Images/tick.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>27</v>
+      </c>
       <c r="C95" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D95" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E95" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F95" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick_large.png</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="16"/>
+        <v>tick_large</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="17"/>
+        <v>tick_large,</v>
+      </c>
+      <c r="F95" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick_large"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>28</v>
+      </c>
       <c r="C96" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D96" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E96" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F96" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick_medium.png</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="16"/>
+        <v>tick_medium</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="17"/>
+        <v>tick_medium,</v>
+      </c>
+      <c r="F96" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>29</v>
+      </c>
       <c r="C97" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D97" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E97" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F97" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick_sharp.png</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="16"/>
+        <v>tick_sharp</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="17"/>
+        <v>tick_sharp,</v>
+      </c>
+      <c r="F97" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick_sharp"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>30</v>
+      </c>
       <c r="C98" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D98" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E98" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F98" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick_sharp_large.png</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="16"/>
+        <v>tick_sharp_large</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="17"/>
+        <v>tick_sharp_large,</v>
+      </c>
+      <c r="F98" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick_sharp_large"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>31</v>
+      </c>
       <c r="C99" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D99" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E99" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F99" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>tick_sharp_medium.png</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="16"/>
+        <v>tick_sharp_medium</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="17"/>
+        <v>tick_sharp_medium,</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="tick_sharp_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/tick_sharp_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
       <c r="C100" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D100" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E100" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F100" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>touch.png</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="16"/>
+        <v>touch</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="17"/>
+        <v>touch,</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="touch"&gt;pack://application:,,,/Haley.WPF;component/Images/touch.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
       <c r="C101" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D101" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E101" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F101" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>touch_large.png</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="16"/>
+        <v>touch_large</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="17"/>
+        <v>touch_large,</v>
+      </c>
+      <c r="F101" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="touch_large"&gt;pack://application:,,,/Haley.WPF;component/Images/touch_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>100</v>
+      </c>
       <c r="C102" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D102" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E102" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F102" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>touch_medium.png</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="16"/>
+        <v>touch_medium</v>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="17"/>
+        <v>touch_medium,</v>
+      </c>
+      <c r="F102" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="touch_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/touch_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
       <c r="C103" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D103" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E103" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F103" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in.png</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in</v>
+      </c>
+      <c r="E103" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in,</v>
+      </c>
+      <c r="F103" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
+        <v>102</v>
+      </c>
       <c r="C104" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D104" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E104" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F104" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in_large.png</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in_large</v>
+      </c>
+      <c r="E104" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in_large,</v>
+      </c>
+      <c r="F104" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in_large"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
       <c r="C105" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D105" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E105" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F105" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in_line.png</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in_line</v>
+      </c>
+      <c r="E105" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in_line,</v>
+      </c>
+      <c r="F105" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in_line"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in_line.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>104</v>
+      </c>
       <c r="C106" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D106" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E106" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F106" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in_line_large.png</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in_line_large</v>
+      </c>
+      <c r="E106" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in_line_large,</v>
+      </c>
+      <c r="F106" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in_line_large"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in_line_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>105</v>
+      </c>
       <c r="C107" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D107" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E107" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F107" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in_line_medium.png</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in_line_medium</v>
+      </c>
+      <c r="E107" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in_line_medium,</v>
+      </c>
+      <c r="F107" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in_line_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in_line_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>106</v>
+      </c>
       <c r="C108" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D108" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E108" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F108" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_in_medium.png</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_in_medium</v>
+      </c>
+      <c r="E108" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_in_medium,</v>
+      </c>
+      <c r="F108" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_in_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_in_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>107</v>
+      </c>
       <c r="C109" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D109" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E109" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F109" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out.png</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out</v>
+      </c>
+      <c r="E109" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out,</v>
+      </c>
+      <c r="F109" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>108</v>
+      </c>
       <c r="C110" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D110" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E110" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F110" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out_large.png</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out_large</v>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out_large,</v>
+      </c>
+      <c r="F110" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out_large"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>109</v>
+      </c>
       <c r="C111" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D111" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E111" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F111" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out_line.png</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out_line</v>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out_line,</v>
+      </c>
+      <c r="F111" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out_line"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out_line.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>110</v>
+      </c>
       <c r="C112" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D112" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E112" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F112" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out_line_large.png</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out_line_large</v>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out_line_large,</v>
+      </c>
+      <c r="F112" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out_line_large"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out_line_large.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>111</v>
+      </c>
       <c r="C113" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D113" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E113" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F113" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out_line_medium.png</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out_line_medium</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out_line_medium,</v>
+      </c>
+      <c r="F113" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out_line_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out_line_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
       <c r="C114" t="str">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="D114" t="e">
-        <f t="shared" si="16"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E114" t="e">
-        <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F114" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+        <v>zoom_out_medium.png</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="16"/>
+        <v>zoom_out_medium</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="17"/>
+        <v>zoom_out_medium,</v>
+      </c>
+      <c r="F114" t="str">
+        <f t="shared" si="18"/>
+        <v>&lt;ImageSource x:Key="zoom_out_medium"&gt;pack://application:,,,/Haley.WPF;component/Images/zoom_out_medium.png&lt;/ImageSource&gt;</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C115" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2523,7 +3009,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C116" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2541,7 +3027,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C117" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2559,7 +3045,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C118" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2577,7 +3063,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C119" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2595,7 +3081,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C120" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2613,7 +3099,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C121" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2631,7 +3117,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C122" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2649,7 +3135,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C123" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2667,7 +3153,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C124" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2685,7 +3171,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C125" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2703,7 +3189,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C126" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2721,7 +3207,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C127" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -2739,7 +3225,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="C128" t="str">
         <f t="shared" si="15"/>
         <v/>

</xml_diff>